<commit_message>
uso del excel durante el procesamiento
</commit_message>
<xml_diff>
--- a/resultados_sunat_detallado.xlsx
+++ b/resultados_sunat_detallado.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Resultados" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,37 +422,37 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>razon_social</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>ruc</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>nombre_encontrado</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>dni_representante</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>nombre_representante</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>cargo</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>fecha_designacion</t>
         </is>
@@ -476,16 +464,11 @@
           <t>SOFIA LIBRERIA Y BAZAR SOCIEDAD COMERCIAL DE RESPONSABILIDAD LIMITADA</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
           <t>No encontrado</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -498,7 +481,6 @@
           <t>20334403166</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
           <t>DNI</t>
@@ -531,7 +513,6 @@
           <t>20334403166</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
           <t>DNI</t>
@@ -564,7 +545,6 @@
           <t>20334403166</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
           <t>DNI</t>
@@ -597,7 +577,6 @@
           <t>20334403166</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
           <t>PASAPORTE</t>
@@ -630,7 +609,6 @@
           <t>20334403166</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
           <t>PASAPORTE</t>
@@ -668,10 +646,6 @@
           <t>baja</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -684,7 +658,6 @@
           <t>20466696065</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
           <t>DNI</t>
@@ -717,7 +690,6 @@
           <t>20603155174</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
           <t>DNI</t>
@@ -750,7 +722,6 @@
           <t>20568169094</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
           <t>DNI</t>
@@ -775,65 +746,58 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>UTILES &amp; MAS LIBRERÍA BAZAR E.I.R.L.</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>20602434045</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>DNI</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>07621087</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>FIGUEROA AYESTA RAFAEL</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>TITULAR-GERENTE</t>
+          <t>SOFIA LIBRERIA Y BAZAR SOCIEDAD COMERCIAL DE RESPONSABILIDAD LIMITADA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>VH FERRETERIA &amp; LIBRERIA SOCIEDAD COMERCIAL DE RESPONSABILIDAD LIMITADA - VH FERRETERIA &amp; LIBRERIA S</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>No encontrado</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
+          <t>SPECIAL BOOK SERVICES S.A.</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>20334403166</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>DNI</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>07378867</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>VASQUEZ VIDAL ROBERTO AMERICO</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>GERENTE DE FINANZAS</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>VQ IMPORTACIONES PERU S.A.C.</t>
+          <t>SPECIAL BOOK SERVICES S.A.</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>20610583947</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr"/>
+          <t>20334403166</t>
+        </is>
+      </c>
       <c r="D14" t="inlineStr">
         <is>
           <t>DNI</t>
@@ -841,32 +805,31 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>70431261</t>
+          <t>08829036</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>QUILLAMA MAYO MELISSA ANN</t>
+          <t>ALVAREZ RIOS DE TAPIA YOLANDA</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>GERENTE GENERAL</t>
+          <t>GERENTE</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>WALAH LIBRERIAS E.I.R.L.</t>
+          <t>SPECIAL BOOK SERVICES S.A.</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>20607658952</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr"/>
+          <t>20334403166</t>
+        </is>
+      </c>
       <c r="D15" t="inlineStr">
         <is>
           <t>DNI</t>
@@ -874,114 +837,397 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>44763901</t>
+          <t>40022471</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>FABIAN HUAMAN CRISTHIAN ALEXANDER</t>
+          <t>BONILLA DEL POZO LUZ JOSEFA</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>GERENTE</t>
+          <t>GERENTE GENERAL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>WINNAAR MV S.R.L.</t>
+          <t>SPECIAL BOOK SERVICES S.A.</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>20608872290</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr"/>
+          <t>20334403166</t>
+        </is>
+      </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>DNI</t>
+          <t>PASAPORTE</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>73104745</t>
+          <t>700620362</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>BARDALES GARCIA VICTOR HUGO</t>
+          <t>ROBERTS TERRY</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>GERENTE</t>
+          <t>DIRECTOR</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>YOKOTA INVERSIONES S.A.C.</t>
+          <t>SPECIAL BOOK SERVICES S.A.</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>20492418367</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr"/>
+          <t>20334403166</t>
+        </is>
+      </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>DNI</t>
+          <t>PASAPORTE</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>07349534</t>
+          <t>X-226792</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>GARCIA YOKOTA DE TAMAYO NELLY ERNESTINA</t>
+          <t>RIBEIRO VICENTE JOSE MAUEL</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>GERENTE GENERAL</t>
+          <t>PRESIDENTE DIRECTORIO</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>SYT COMPANY S.A.C.</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>baja</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>baja</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>TATI Y DEYANIRA LIBRERIA BAZAR S.R.L.</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>20466696065</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>DNI</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>07709939</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>PLAZARTE ALEJANDRO LEONOR BLANCA</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>GERENTE GENERAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>TONINA E.I.R.L.</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>20603155174</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>DNI</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>07635120</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>LAZARO MEJIA ANTUHANETT</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>TITULAR-GERENTE</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>UNIVERSO EMPRESARIAL S.A.C.</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>20568169094</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>DNI</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>19863031</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>MENDOZA POVES LUZ SOCORRO</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>GERENTE GENERAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>UTILES &amp; MAS LIBRERÍA BAZAR E.I.R.L.</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>20602434045</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>DNI</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>07621087</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>FIGUEROA AYESTA RAFAEL</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>TITULAR-GERENTE</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>VH FERRETERIA &amp; LIBRERIA SOCIEDAD COMERCIAL DE RESPONSABILIDAD LIMITADA - VH FERRETERIA &amp; LIBRERIA S</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>No encontrado</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>VQ IMPORTACIONES PERU S.A.C.</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>20610583947</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>DNI</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>70431261</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>QUILLAMA MAYO MELISSA ANN</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>GERENTE GENERAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>WALAH LIBRERIAS E.I.R.L.</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>20607658952</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>DNI</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>44763901</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>FABIAN HUAMAN CRISTHIAN ALEXANDER</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>GERENTE</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>WINNAAR MV S.R.L.</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>20608872290</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>DNI</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>73104745</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>BARDALES GARCIA VICTOR HUGO</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>GERENTE</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>YOKOTA INVERSIONES S.A.C.</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>20492418367</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>DNI</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>07349534</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>GARCIA YOKOTA DE TAMAYO NELLY ERNESTINA</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>GERENTE GENERAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
           <t>YOVIS C &amp; M LIBRERIA Y ACCESORIOS E.I.R.L.</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B28" t="inlineStr">
         <is>
           <t>20612686611</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>DNI</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>DNI</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
         <is>
           <t>40820117</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>CUSI MAMANI YOVANA ELSI</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="G28" t="inlineStr">
         <is>
           <t>TITULAR-GERENTE</t>
         </is>

</xml_diff>